<commit_message>
added but error with identity
</commit_message>
<xml_diff>
--- a/STUDY.ConsoleP.ExcelReader/STUDY.ConsoleP.ExcelReader/ExcelReaderData.xlsx
+++ b/STUDY.ConsoleP.ExcelReader/STUDY.ConsoleP.ExcelReader/ExcelReaderData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MEGA\WIP\01-GitClone\STUDY.ConsoleP.ExcelReader\STUDY.ConsoleP.ExcelReader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MEGA\WIP\02-GitWIP\STUDY.ConsoleP.ExcelReader\STUDY.ConsoleP.ExcelReader\STUDY.ConsoleP.ExcelReader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395CDE08-B6E5-48A1-910E-1163C4199FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA564767-EC68-4F1B-8AB3-4F5E7C53456A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8CE46605-FFB9-4833-9ABB-A788CF72837C}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -52,6 +49,9 @@
   </si>
   <si>
     <t>Huang</t>
+  </si>
+  <si>
+    <t>Id</t>
   </si>
 </sst>
 </file>
@@ -406,7 +406,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,13 +417,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -431,10 +431,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -442,10 +442,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -453,10 +453,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>